<commit_message>
Fix for students who request no one
</commit_message>
<xml_diff>
--- a/Real2020Entry1/forBot_FacultyAvailabilityMatrix.xlsx
+++ b/Real2020Entry1/forBot_FacultyAvailabilityMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/Real2020Entry1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6102DD-0452-EE47-BDC0-EE839D4591AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154A3C8F-6675-5249-8196-8D99D68303F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="13480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,56 +38,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
   <si>
     <t>Scott Atwood</t>
   </si>
   <si>
-    <t>Bardwell</t>
-  </si>
-  <si>
-    <t>Brody</t>
-  </si>
-  <si>
     <t>Ken Cho</t>
   </si>
   <si>
     <t>Steve Frank</t>
   </si>
   <si>
-    <t>Lander</t>
+    <t>Komarova</t>
   </si>
   <si>
     <t>Chang Liu</t>
   </si>
   <si>
-    <t>Mortazavi</t>
-  </si>
-  <si>
     <t>Qing Nie</t>
   </si>
   <si>
-    <t>Ranz</t>
-  </si>
-  <si>
-    <t>Siryaporn</t>
+    <t>Read</t>
   </si>
   <si>
     <t>Knut Solna</t>
   </si>
   <si>
-    <t>Swarup</t>
-  </si>
-  <si>
-    <t>Whiteson</t>
-  </si>
-  <si>
-    <t>Wodarz</t>
-  </si>
-  <si>
-    <t>Wunderlich</t>
-  </si>
-  <si>
     <t>Jack Xin</t>
   </si>
   <si>
@@ -160,6 +136,9 @@
     <t>Jun Allard</t>
   </si>
   <si>
+    <t>John Lowengrub</t>
+  </si>
+  <si>
     <t>Ilhem Messaoudi</t>
   </si>
   <si>
@@ -196,15 +175,9 @@
     <t xml:space="preserve">Downing </t>
   </si>
   <si>
-    <t>Schilling</t>
-  </si>
-  <si>
     <t>Joyce Keyak</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>440 F Rowland Hall #949/824-1954</t>
   </si>
   <si>
@@ -230,6 +203,129 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>James Brody</t>
+  </si>
+  <si>
+    <t>Lee Bardwell</t>
+  </si>
+  <si>
+    <t>463 Steinhaus Hall #949/824-2061</t>
+  </si>
+  <si>
+    <t>3102 BioSci 3 #949/824-2244</t>
+  </si>
+  <si>
+    <t>2418 Engineering 3 #949/824-3211</t>
+  </si>
+  <si>
+    <t>4092 Bren Hall #949/824-1753</t>
+  </si>
+  <si>
+    <t>2600 BioSci 3 #949/824-1721</t>
+  </si>
+  <si>
+    <t>Arthur Lander</t>
+  </si>
+  <si>
+    <t>112 Sprague Hall #949/824-2991</t>
+  </si>
+  <si>
+    <t>5207 McGaugh Hall</t>
+  </si>
+  <si>
+    <t>3105 NatSci 2 #949/824-8534</t>
+  </si>
+  <si>
+    <t>540 H Rowland Hall #949/824-8456</t>
+  </si>
+  <si>
+    <t>2216 BioSci 3 #949/824-3078</t>
+  </si>
+  <si>
+    <t>5232 McGaugh Hall #949/302-7325</t>
+  </si>
+  <si>
+    <t>Ali Mortazavi</t>
+  </si>
+  <si>
+    <t>2218 BioSci 3 #949/824-6762</t>
+  </si>
+  <si>
+    <t>540F Rowland Hall #949/824-5530</t>
+  </si>
+  <si>
+    <t>1107 NatSci 2 #949/824-9942</t>
+  </si>
+  <si>
+    <t>456 Steinhaus Hall #949/824-9071</t>
+  </si>
+  <si>
+    <t>4109 NatSci 2 #949/824-2479</t>
+  </si>
+  <si>
+    <t>314 Sprague Hall #949/824-6765</t>
+  </si>
+  <si>
+    <t>Jose Ranz</t>
+  </si>
+  <si>
+    <t>Thomas Schilling</t>
+  </si>
+  <si>
+    <t>Albert Siryaporn</t>
+  </si>
+  <si>
+    <t>210C Rowland Hall #949/824-5141</t>
+  </si>
+  <si>
+    <t>540 G Rowland Hall #949/824-3154</t>
+  </si>
+  <si>
+    <t>Vivek Swarup</t>
+  </si>
+  <si>
+    <t>3224 BioSci 3 #949/824-3182</t>
+  </si>
+  <si>
+    <t>3110 BioSci 3 #949/824-3120</t>
+  </si>
+  <si>
+    <t>3036 Hewitt Hall #949/824-6150</t>
+  </si>
+  <si>
+    <t>Katrine Whiteson</t>
+  </si>
+  <si>
+    <t>3236 McGaugh Hall #949/824-9032</t>
+  </si>
+  <si>
+    <t>Dominik Wodarz</t>
+  </si>
+  <si>
+    <t>2072 AIRB #949/824-2531</t>
+  </si>
+  <si>
+    <t>Zeba Wunderlich</t>
+  </si>
+  <si>
+    <t>4107 NatSci 2 #949/824-5959</t>
+  </si>
+  <si>
+    <t>540E Rowland Hall #949/824-5309</t>
+  </si>
+  <si>
+    <t>H128 Hitachi Bldg #949/824-8215</t>
+  </si>
+  <si>
+    <t>220B Rowland Hall #949/824-2177</t>
+  </si>
+  <si>
+    <t>Enciso</t>
+  </si>
+  <si>
+    <t>Clare</t>
   </si>
 </sst>
 </file>
@@ -312,7 +408,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -361,22 +457,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,9 +537,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,17 +548,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,11 +868,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ16"/>
+  <dimension ref="A1:AM15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK15" sqref="AK15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,184 +886,264 @@
     <col min="7" max="7" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
     <col min="15" max="16" width="15.5" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" style="21" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" customWidth="1"/>
-    <col min="25" max="25" width="13" customWidth="1"/>
-    <col min="29" max="29" width="11.83203125" customWidth="1"/>
-    <col min="35" max="35" width="17.33203125" customWidth="1"/>
-    <col min="36" max="36" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="21" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.5" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="16.83203125" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" customWidth="1"/>
+    <col min="31" max="31" width="14" customWidth="1"/>
+    <col min="32" max="32" width="15.33203125" customWidth="1"/>
+    <col min="33" max="33" width="14.83203125" customWidth="1"/>
+    <col min="34" max="34" width="14.1640625" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" customWidth="1"/>
+    <col min="36" max="36" width="17.33203125" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="23" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="L1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+    </row>
+    <row r="2" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" s="22" t="s">
+      <c r="F2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC2" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK2" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC1" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF1" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ1" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="26"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
       <c r="C3" s="3">
@@ -999,7 +1155,7 @@
       <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="13">
         <v>1</v>
       </c>
@@ -1013,41 +1169,46 @@
       <c r="O3" s="18"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="16"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="2"/>
+      <c r="R3" s="3">
+        <v>1</v>
+      </c>
+      <c r="S3" s="20"/>
+      <c r="T3" s="3"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="3">
-        <v>1</v>
-      </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="12"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="3"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3">
+        <v>1</v>
+      </c>
       <c r="AH3" s="3"/>
-      <c r="AI3" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="18"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1075,45 +1236,50 @@
       <c r="O4" s="18"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="2"/>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="20"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="12">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="12">
         <v>1</v>
       </c>
       <c r="Y4" s="2">
         <v>1</v>
       </c>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="2"/>
+      <c r="Z4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2">
+        <v>1</v>
+      </c>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1143,53 +1309,58 @@
       <c r="O5" s="18"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
-        <v>1</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2">
-        <v>1</v>
-      </c>
-      <c r="W5" s="12">
-        <v>1</v>
-      </c>
-      <c r="X5" s="2">
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="20"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="12">
         <v>1</v>
       </c>
       <c r="Y5" s="2">
         <v>1</v>
       </c>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="2">
+      <c r="Z5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="12">
         <v>1</v>
       </c>
       <c r="AD5" s="2">
         <v>1</v>
       </c>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2">
-        <v>1</v>
-      </c>
+      <c r="AE5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2"/>
       <c r="AG5" s="2">
         <v>1</v>
       </c>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AH5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1217,55 +1388,58 @@
         <v>1</v>
       </c>
       <c r="Q6" s="8"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2">
-        <v>1</v>
-      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="2"/>
       <c r="U6" s="2">
         <v>1</v>
       </c>
       <c r="V6" s="2">
         <v>1</v>
       </c>
-      <c r="W6" s="12">
-        <v>1</v>
-      </c>
-      <c r="X6" s="2">
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="12">
         <v>1</v>
       </c>
       <c r="Y6" s="2">
         <v>1</v>
       </c>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="2">
-        <v>1</v>
-      </c>
+      <c r="Z6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="7"/>
       <c r="AC6" s="2">
         <v>1</v>
       </c>
       <c r="AD6" s="2">
         <v>1</v>
       </c>
-      <c r="AE6" s="2"/>
+      <c r="AE6" s="2">
+        <v>1</v>
+      </c>
       <c r="AF6" s="2"/>
-      <c r="AG6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="18"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -1289,51 +1463,54 @@
       <c r="Q7" s="11">
         <v>1</v>
       </c>
-      <c r="R7" s="20"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2">
-        <v>1</v>
-      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2"/>
       <c r="Y7" s="2">
         <v>1</v>
       </c>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="2"/>
       <c r="AC7" s="2">
         <v>1</v>
       </c>
       <c r="AD7" s="2">
         <v>1</v>
       </c>
-      <c r="AE7" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="2"/>
+      <c r="AE7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="12">
+        <v>1</v>
+      </c>
       <c r="AG7" s="2"/>
-      <c r="AH7" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="18"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -1357,45 +1534,48 @@
       <c r="Q8" s="12">
         <v>1</v>
       </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="12">
-        <v>1</v>
-      </c>
-      <c r="U8" s="2"/>
-      <c r="V8" s="11">
-        <v>1</v>
-      </c>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="4"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ8" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="R8" s="4"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="12">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="11">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="11">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1433,47 +1613,52 @@
       <c r="Q9" s="12">
         <v>1</v>
       </c>
-      <c r="R9" s="9">
-        <v>1</v>
-      </c>
-      <c r="S9" s="2">
-        <v>1</v>
-      </c>
-      <c r="T9" s="2"/>
+      <c r="R9" s="2">
+        <v>1</v>
+      </c>
+      <c r="S9" s="9">
+        <v>1</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1</v>
+      </c>
       <c r="U9" s="2"/>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
-      <c r="W9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
       <c r="X9" s="2"/>
-      <c r="Y9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="6"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="2">
-        <v>1</v>
-      </c>
+      <c r="AD9" s="2"/>
       <c r="AE9" s="2">
         <v>1</v>
       </c>
       <c r="AF9" s="2">
         <v>1</v>
       </c>
-      <c r="AG9" s="2"/>
+      <c r="AG9" s="2">
+        <v>1</v>
+      </c>
       <c r="AH9" s="2"/>
-      <c r="AI9" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -1505,31 +1690,31 @@
       <c r="O10" s="18"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="12"/>
-      <c r="R10" s="11">
-        <v>1</v>
-      </c>
-      <c r="S10" s="2">
-        <v>1</v>
-      </c>
-      <c r="T10" s="2"/>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="S10" s="11">
+        <v>1</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1</v>
+      </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
-      <c r="Y10" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="2">
-        <v>1</v>
-      </c>
+      <c r="AD10" s="2"/>
       <c r="AE10" s="2">
         <v>1</v>
       </c>
@@ -1539,17 +1724,22 @@
       <c r="AG10" s="2">
         <v>1</v>
       </c>
-      <c r="AH10" s="2"/>
-      <c r="AI10" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AH10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="18"/>
+      <c r="AM10" s="18"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
@@ -1579,26 +1769,26 @@
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="11">
-        <v>1</v>
-      </c>
-      <c r="S11" s="2">
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+      <c r="S11" s="11">
         <v>1</v>
       </c>
       <c r="T11" s="2">
         <v>1</v>
       </c>
-      <c r="U11" s="2"/>
+      <c r="U11" s="2">
+        <v>1</v>
+      </c>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
-      <c r="Y11" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="2">
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="12">
         <v>1</v>
       </c>
       <c r="AB11" s="2">
@@ -1610,22 +1800,27 @@
       <c r="AD11" s="2">
         <v>1</v>
       </c>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="2"/>
+      <c r="AE11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2">
+        <v>1</v>
+      </c>
       <c r="AH11" s="2"/>
-      <c r="AI11" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -1634,8 +1829,8 @@
       <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>54</v>
+      <c r="E12" s="2">
+        <v>1</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="2"/>
@@ -1657,31 +1852,31 @@
         <v>1</v>
       </c>
       <c r="Q12" s="12"/>
-      <c r="R12" s="11">
-        <v>1</v>
-      </c>
-      <c r="S12" s="2">
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+      <c r="S12" s="11">
         <v>1</v>
       </c>
       <c r="T12" s="2">
         <v>1</v>
       </c>
-      <c r="U12" s="12">
-        <v>1</v>
-      </c>
-      <c r="V12" s="2"/>
+      <c r="U12" s="2">
+        <v>1</v>
+      </c>
+      <c r="V12" s="12">
+        <v>1</v>
+      </c>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="12">
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2">
         <v>1</v>
       </c>
       <c r="AA12" s="12">
         <v>1</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AB12" s="12">
         <v>1</v>
       </c>
       <c r="AC12" s="2">
@@ -1690,20 +1885,25 @@
       <c r="AD12" s="2">
         <v>1</v>
       </c>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="4"/>
+      <c r="AE12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="2"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -1712,8 +1912,8 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>54</v>
+      <c r="E13" s="2">
+        <v>1</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="2"/>
@@ -1737,26 +1937,24 @@
         <v>1</v>
       </c>
       <c r="Q13" s="12"/>
-      <c r="R13" s="11">
-        <v>1</v>
-      </c>
-      <c r="S13" s="2">
+      <c r="R13" s="2"/>
+      <c r="S13" s="11">
         <v>1</v>
       </c>
       <c r="T13" s="2">
         <v>1</v>
       </c>
-      <c r="U13" s="2"/>
+      <c r="U13" s="2">
+        <v>1</v>
+      </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
-      <c r="Y13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="2">
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="12">
         <v>1</v>
       </c>
       <c r="AB13" s="2">
@@ -1768,28 +1966,33 @@
       <c r="AD13" s="2">
         <v>1</v>
       </c>
-      <c r="AE13" s="2"/>
+      <c r="AE13" s="2">
+        <v>1</v>
+      </c>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
-      <c r="AI13" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="18"/>
+      <c r="AM13" s="18"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>54</v>
+      <c r="E14" s="2">
+        <v>1</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="2"/>
@@ -1809,83 +2012,109 @@
         <v>1</v>
       </c>
       <c r="Q14" s="12"/>
-      <c r="R14" s="11">
-        <v>1</v>
-      </c>
+      <c r="R14" s="4"/>
       <c r="S14" s="11">
         <v>1</v>
       </c>
-      <c r="T14" s="12">
-        <v>1</v>
-      </c>
-      <c r="U14" s="2"/>
+      <c r="T14" s="11">
+        <v>1</v>
+      </c>
+      <c r="U14" s="12">
+        <v>1</v>
+      </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
-      <c r="Y14" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="12"/>
       <c r="AB14" s="2">
         <v>1</v>
       </c>
-      <c r="AC14" s="11">
+      <c r="AC14" s="2">
         <v>1</v>
       </c>
       <c r="AD14" s="11">
         <v>1</v>
       </c>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="4"/>
+      <c r="AE14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="2"/>
       <c r="AG14" s="4"/>
       <c r="AH14" s="4"/>
-      <c r="AI14" s="17">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="33">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="O15" s="33">
-        <v>1</v>
-      </c>
-      <c r="P15" s="33">
-        <v>1</v>
-      </c>
-      <c r="R15" s="21">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="33">
-        <v>1</v>
-      </c>
-      <c r="AE15">
-        <v>1</v>
-      </c>
-      <c r="AG15">
-        <v>1</v>
-      </c>
-      <c r="AI15" s="34">
-        <v>1</v>
-      </c>
-      <c r="AJ15" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="J16" s="32"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="18"/>
+      <c r="AM14" s="18"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="17">
+        <v>1</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="17">
+        <v>1</v>
+      </c>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="17">
+        <v>1</v>
+      </c>
+      <c r="P15" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="17">
+        <v>1</v>
+      </c>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="17">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="17">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="17">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1895,43 +2124,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C34A2F6-03A8-4A9E-97C6-B9E492BDE22D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>53</v>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I13" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I14" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I15" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I18" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="I24" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="I38" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I41" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I42" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>